<commit_message>
eval step by step
</commit_message>
<xml_diff>
--- a/scripts/baseline/baseline_bert_supervised.xlsx
+++ b/scripts/baseline/baseline_bert_supervised.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -357,17 +357,17 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,7 +387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -407,7 +407,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -427,7 +427,7 @@
         <v>25.45</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -447,7 +447,7 @@
         <v>27.58</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -467,7 +467,7 @@
         <v>24.73</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -487,7 +487,7 @@
         <v>30.18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -507,7 +507,7 @@
         <v>26.32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -527,7 +527,7 @@
         <v>33.229999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -547,7 +547,7 @@
         <v>29.53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -567,7 +567,7 @@
         <v>31.39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -587,7 +587,7 @@
         <v>35.619999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -607,7 +607,7 @@
         <v>31.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>15</v>
       </c>
@@ -627,7 +627,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>20</v>
       </c>
@@ -647,7 +647,7 @@
         <v>33.18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>25</v>
       </c>
@@ -667,7 +667,7 @@
         <v>31.77</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>30</v>
       </c>
@@ -687,7 +687,7 @@
         <v>35.409999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>35</v>
       </c>
@@ -707,7 +707,7 @@
         <v>33.69</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>40</v>
       </c>
@@ -727,7 +727,7 @@
         <v>33.15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>45</v>
       </c>
@@ -747,7 +747,7 @@
         <v>36.32</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>50</v>
       </c>
@@ -767,7 +767,7 @@
         <v>37.590000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>60</v>
       </c>
@@ -787,7 +787,7 @@
         <v>36.49</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>70</v>
       </c>
@@ -807,7 +807,7 @@
         <v>35.01</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>80</v>
       </c>
@@ -827,7 +827,7 @@
         <v>37.04</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>90</v>
       </c>

</xml_diff>